<commit_message>
Typ sensor RJ-45 includes limit, pos and A/B
</commit_message>
<xml_diff>
--- a/Wiring.xlsx
+++ b/Wiring.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27380" yWindow="13200" windowWidth="41300" windowHeight="23800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="41">
   <si>
     <t>RJ-45</t>
   </si>
@@ -62,12 +62,6 @@
     <t>White</t>
   </si>
   <si>
-    <t>B Chan</t>
-  </si>
-  <si>
-    <t>A Chan</t>
-  </si>
-  <si>
     <t>Green</t>
   </si>
   <si>
@@ -128,21 +122,9 @@
     <t>DIO-n (sig)</t>
   </si>
   <si>
-    <t xml:space="preserve"> up limit</t>
-  </si>
-  <si>
-    <t>down limit</t>
-  </si>
-  <si>
-    <t>Typical Limit Switch / Potentiometer</t>
-  </si>
-  <si>
     <t>AIO-n (sig)</t>
   </si>
   <si>
-    <t>position</t>
-  </si>
-  <si>
     <t>Rockwell 42JS Photoelectric Sensor</t>
   </si>
   <si>
@@ -150,6 +132,24 @@
   </si>
   <si>
     <t>dark out</t>
+  </si>
+  <si>
+    <t>Typical Limit Switch / Potentiometer / Encoder</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -251,9 +251,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -270,6 +267,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -602,7 +602,7 @@
   <dimension ref="B4:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="Y30" sqref="Y30"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,24 +632,24 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:22" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
       <c r="G4" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="K4" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
       <c r="O4" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
@@ -667,13 +667,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>26</v>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>7</v>
@@ -681,8 +681,8 @@
       <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>26</v>
+      <c r="K5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>7</v>
@@ -690,8 +690,8 @@
       <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>26</v>
+      <c r="O5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>7</v>
@@ -700,8 +700,8 @@
         <v>8</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="5" t="s">
-        <v>26</v>
+      <c r="S5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>7</v>
@@ -729,49 +729,44 @@
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="R7" s="3"/>
       <c r="S7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
@@ -780,49 +775,44 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="I8" s="1"/>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
@@ -831,28 +821,36 @@
       <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="I9" s="1"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="1"/>
+      <c r="K9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="M9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -861,22 +859,41 @@
       <c r="B10" s="1">
         <v>4</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
+      <c r="S10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
@@ -884,27 +901,43 @@
       <c r="B11" s="1">
         <v>5</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
+      <c r="S11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
@@ -912,14 +945,14 @@
       <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="1"/>
@@ -928,10 +961,10 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="O12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>9</v>
@@ -946,42 +979,42 @@
       <c r="B13" s="1">
         <v>7</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
@@ -990,7 +1023,7 @@
       <c r="B14" s="1">
         <v>8</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1003,7 +1036,7 @@
         <v>3</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>9</v>
@@ -1012,26 +1045,26 @@
         <v>3</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>

</xml_diff>

<commit_message>
Add encoder DIO assignments
</commit_message>
<xml_diff>
--- a/Wiring.xlsx
+++ b/Wiring.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="45">
   <si>
     <t>RJ-45</t>
   </si>
@@ -150,6 +150,18 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>DIO-0 (sig)</t>
+  </si>
+  <si>
+    <t>DIO-1 (sig)</t>
+  </si>
+  <si>
+    <t>DIO-2 (sig)</t>
+  </si>
+  <si>
+    <t>DIO-3 (sig)</t>
   </si>
 </sst>
 </file>
@@ -602,7 +614,7 @@
   <dimension ref="B4:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="R1" sqref="R1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,21 +624,21 @@
     <col min="3" max="3" width="5" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.83203125" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2.83203125" customWidth="1"/>
     <col min="11" max="11" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.6640625" customWidth="1"/>
     <col min="18" max="18" width="2.6640625" customWidth="1"/>
     <col min="19" max="19" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="2.6640625" customWidth="1"/>
   </cols>
@@ -639,22 +651,22 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="G4" s="11" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="K4" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
       <c r="O4" s="11" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="11"/>
       <c r="S4" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
@@ -672,7 +684,8 @@
       <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -681,7 +694,7 @@
       <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="5" t="s">
         <v>24</v>
       </c>
       <c r="L5" s="1" t="s">
@@ -699,7 +712,6 @@
       <c r="Q5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="1"/>
       <c r="S5" s="4" t="s">
         <v>24</v>
       </c>
@@ -712,14 +724,14 @@
       <c r="V5" s="1"/>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
@@ -738,37 +750,29 @@
       <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="K7" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="2"/>
       <c r="L7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="M7" s="1"/>
       <c r="P7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="U7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="R7" s="3"/>
-      <c r="S7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="U7" s="3"/>
       <c r="V7" s="3"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.2">
@@ -784,7 +788,7 @@
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
         <v>30</v>
       </c>
@@ -792,29 +796,21 @@
         <v>37</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="K8" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="J8" s="2"/>
       <c r="L8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="M8" s="1"/>
       <c r="P8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="U8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.2">
@@ -830,6 +826,7 @@
       <c r="E9" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
         <v>31</v>
       </c>
@@ -837,21 +834,14 @@
         <v>38</v>
       </c>
       <c r="I9" s="1"/>
-      <c r="K9" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="L9" s="1" t="s">
         <v>38</v>
       </c>
       <c r="M9" s="1"/>
+      <c r="P9" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
@@ -868,17 +858,16 @@
       <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="I10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>39</v>
@@ -886,13 +875,14 @@
       <c r="M10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T10" s="1" t="s">
+      <c r="O10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
@@ -910,17 +900,16 @@
       <c r="E11" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="I11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>40</v>
@@ -928,16 +917,17 @@
       <c r="M11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T11" s="1" t="s">
+      <c r="O11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="Q11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
@@ -954,25 +944,25 @@
       <c r="E12" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="1"/>
       <c r="K12" s="3"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="3"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="S12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="T12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="U12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R12" s="1"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.2">
@@ -988,15 +978,14 @@
       <c r="E13" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="I13" s="1"/>
       <c r="K13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1006,16 +995,17 @@
       <c r="M13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="3"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="T13" s="3" t="s">
+      <c r="P13" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="Q13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
@@ -1032,15 +1022,14 @@
       <c r="E14" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="I14" s="1"/>
       <c r="K14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1051,83 +1040,84 @@
         <v>9</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R14" s="1"/>
+        <v>9</v>
+      </c>
       <c r="S14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U14" s="1"/>
+      <c r="U14" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="V14" s="1"/>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G18"/>
+    <row r="18" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K18"/>
-    </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G19"/>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K19"/>
-    </row>
-    <row r="20" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G20"/>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K20"/>
-    </row>
-    <row r="21" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G21"/>
+      <c r="O20"/>
+    </row>
+    <row r="21" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K21"/>
-    </row>
-    <row r="22" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G22"/>
+      <c r="O21"/>
+    </row>
+    <row r="22" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K22"/>
-    </row>
-    <row r="23" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="G23"/>
+      <c r="O22"/>
+    </row>
+    <row r="23" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K23"/>
-    </row>
-    <row r="24" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="H28" s="3"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="7:11" x14ac:dyDescent="0.2">
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
+      <c r="O23"/>
+    </row>
+    <row r="24" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="L28" s="3"/>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B4:E4"/>
+    <mergeCell ref="S4:U4"/>
     <mergeCell ref="O4:Q4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="G4:I4"/>
-    <mergeCell ref="S4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>